<commit_message>
CI: pretas may 2021 - wip
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/May 2021/ci_lf_pretas_1_site_202105.xlsx
+++ b/LF/PreTAS/Ivory Coast/May 2021/ci_lf_pretas_1_site_202105.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\May 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562996D3-0A6F-4705-96A2-EE21D4650BE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2CD5DB-9382-45A5-8FB8-9872889EDAA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -681,9 +681,6 @@
     <t>ci_lf_pretas_1_site_202105_v2</t>
   </si>
   <si>
-    <t>1. Côte d'Ivoire - Pre TAS FL Fromulaire Site V2</t>
-  </si>
-  <si>
     <t>Autre</t>
   </si>
   <si>
@@ -955,6 +952,9 @@
   </si>
   <si>
     <t>Type Dest</t>
+  </si>
+  <si>
+    <t>(May 2021) 1. Côte d'Ivoire - Pre TAS FL Fromulaire Site V2</t>
   </si>
 </sst>
 </file>
@@ -1377,11 +1377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1627,11 +1627,11 @@
         <v>205</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="8"/>
@@ -1639,7 +1639,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="4" t="s">
@@ -1656,22 +1656,22 @@
         <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>290</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E9" t="s">
+        <v>284</v>
+      </c>
+      <c r="F9" t="s">
         <v>285</v>
       </c>
-      <c r="F9" t="s">
-        <v>286</v>
-      </c>
       <c r="K9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M9" t="s">
         <v>56</v>
@@ -1679,25 +1679,25 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E10" t="s">
         <v>291</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
+        <v>286</v>
+      </c>
+      <c r="K10" t="s">
         <v>301</v>
-      </c>
-      <c r="E10" t="s">
-        <v>292</v>
-      </c>
-      <c r="F10" t="s">
-        <v>287</v>
-      </c>
-      <c r="K10" t="s">
-        <v>302</v>
       </c>
       <c r="M10" t="s">
         <v>56</v>
@@ -1795,14 +1795,14 @@
         <v>45</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>295</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>296</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1939,8 +1939,8 @@
   <dimension ref="A1:H323"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J258" sqref="J258:K323"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A258" sqref="A258:F323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4275,13 +4275,13 @@
         <v>44</v>
       </c>
       <c r="B124" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C124" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D124" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="12" t="s">
@@ -4296,13 +4296,13 @@
         <v>44</v>
       </c>
       <c r="B125" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C125" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D125" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E125" s="7"/>
       <c r="F125" s="12" t="s">
@@ -4317,13 +4317,13 @@
         <v>44</v>
       </c>
       <c r="B126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E126" s="7"/>
       <c r="F126" s="12" t="s">
@@ -4338,13 +4338,13 @@
         <v>44</v>
       </c>
       <c r="B127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E127" s="7"/>
       <c r="F127" s="12" t="s">
@@ -4359,13 +4359,13 @@
         <v>44</v>
       </c>
       <c r="B128" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C128" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D128" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="12" t="s">
@@ -4380,13 +4380,13 @@
         <v>44</v>
       </c>
       <c r="B129" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C129" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D129" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E129" s="7"/>
       <c r="F129" s="12" t="s">
@@ -4401,13 +4401,13 @@
         <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C130" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D130" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E130" s="7"/>
       <c r="F130" s="12" t="s">
@@ -4422,13 +4422,13 @@
         <v>44</v>
       </c>
       <c r="B131" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C131" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D131" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E131" s="7"/>
       <c r="F131" s="12" t="s">
@@ -4443,13 +4443,13 @@
         <v>44</v>
       </c>
       <c r="B132" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C132" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D132" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E132" s="7"/>
       <c r="F132" s="12" t="s">
@@ -4464,13 +4464,13 @@
         <v>44</v>
       </c>
       <c r="B133" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C133" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D133" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E133" s="7"/>
       <c r="F133" s="12" t="s">
@@ -4485,13 +4485,13 @@
         <v>44</v>
       </c>
       <c r="B134" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C134" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D134" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E134" s="7"/>
       <c r="F134" s="12" t="s">
@@ -4506,13 +4506,13 @@
         <v>44</v>
       </c>
       <c r="B135" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C135" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D135" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E135" s="7"/>
       <c r="F135" s="12" t="s">
@@ -4527,13 +4527,13 @@
         <v>44</v>
       </c>
       <c r="B136" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C136" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D136" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E136" s="7"/>
       <c r="F136" s="12" t="s">
@@ -4548,13 +4548,13 @@
         <v>44</v>
       </c>
       <c r="B137" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C137" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D137" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="12" t="s">
@@ -4569,13 +4569,13 @@
         <v>44</v>
       </c>
       <c r="B138" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C138" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D138" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E138" s="7"/>
       <c r="F138" s="12" t="s">
@@ -4590,13 +4590,13 @@
         <v>44</v>
       </c>
       <c r="B139" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C139" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D139" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" s="12" t="s">
@@ -4611,13 +4611,13 @@
         <v>44</v>
       </c>
       <c r="B140" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C140" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D140" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E140" s="7"/>
       <c r="F140" s="12" t="s">
@@ -4632,13 +4632,13 @@
         <v>44</v>
       </c>
       <c r="B141" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C141" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D141" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="12" t="s">
@@ -4653,13 +4653,13 @@
         <v>44</v>
       </c>
       <c r="B142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E142" s="7"/>
       <c r="F142" s="12" t="s">
@@ -4674,13 +4674,13 @@
         <v>44</v>
       </c>
       <c r="B143" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C143" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D143" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E143" s="7"/>
       <c r="F143" s="12" t="s">
@@ -4695,13 +4695,13 @@
         <v>44</v>
       </c>
       <c r="B144" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C144" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D144" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E144" s="7"/>
       <c r="F144" s="12" t="s">
@@ -4716,13 +4716,13 @@
         <v>44</v>
       </c>
       <c r="B145" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C145" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D145" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="12" t="s">
@@ -4737,13 +4737,13 @@
         <v>44</v>
       </c>
       <c r="B146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E146" s="7"/>
       <c r="F146" s="12" t="s">
@@ -4758,13 +4758,13 @@
         <v>44</v>
       </c>
       <c r="B147" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C147" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D147" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E147" s="7"/>
       <c r="F147" s="12" t="s">
@@ -4779,13 +4779,13 @@
         <v>44</v>
       </c>
       <c r="B148" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C148" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D148" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E148" s="7"/>
       <c r="F148" s="12" t="s">
@@ -4800,13 +4800,13 @@
         <v>44</v>
       </c>
       <c r="B149" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C149" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D149" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E149" s="7"/>
       <c r="F149" s="12" t="s">
@@ -4821,13 +4821,13 @@
         <v>44</v>
       </c>
       <c r="B150" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C150" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D150" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E150" s="7"/>
       <c r="F150" s="12" t="s">
@@ -4842,13 +4842,13 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C151" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D151" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E151" s="7"/>
       <c r="F151" s="12" t="s">
@@ -4863,13 +4863,13 @@
         <v>44</v>
       </c>
       <c r="B152" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C152" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D152" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E152" s="7"/>
       <c r="F152" s="12" t="s">
@@ -4884,13 +4884,13 @@
         <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C153" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D153" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E153" s="7"/>
       <c r="F153" s="12" t="s">
@@ -4905,13 +4905,13 @@
         <v>44</v>
       </c>
       <c r="B154" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C154" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D154" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E154" s="7"/>
       <c r="F154" s="12" t="s">
@@ -4926,13 +4926,13 @@
         <v>44</v>
       </c>
       <c r="B155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E155" s="7"/>
       <c r="F155" s="12" t="s">
@@ -4947,13 +4947,13 @@
         <v>44</v>
       </c>
       <c r="B156" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C156" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D156" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E156" s="7"/>
       <c r="F156" s="12" t="s">
@@ -4968,13 +4968,13 @@
         <v>44</v>
       </c>
       <c r="B157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E157" s="7"/>
       <c r="F157" s="12" t="s">
@@ -4989,13 +4989,13 @@
         <v>44</v>
       </c>
       <c r="B158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E158" s="7"/>
       <c r="F158" s="12" t="s">
@@ -5010,13 +5010,13 @@
         <v>44</v>
       </c>
       <c r="B159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E159" s="7"/>
       <c r="F159" s="12" t="s">
@@ -5031,13 +5031,13 @@
         <v>44</v>
       </c>
       <c r="B160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E160" s="7"/>
       <c r="F160" s="12" t="s">
@@ -5052,13 +5052,13 @@
         <v>44</v>
       </c>
       <c r="B161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E161" s="7"/>
       <c r="F161" s="12" t="s">
@@ -5073,13 +5073,13 @@
         <v>44</v>
       </c>
       <c r="B162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E162" s="7"/>
       <c r="F162" s="12" t="s">
@@ -5094,13 +5094,13 @@
         <v>44</v>
       </c>
       <c r="B163" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C163" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D163" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E163" s="7"/>
       <c r="F163" s="12" t="s">
@@ -5115,13 +5115,13 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C164" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D164" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E164" s="7"/>
       <c r="F164" s="12" t="s">
@@ -5136,13 +5136,13 @@
         <v>44</v>
       </c>
       <c r="B165" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C165" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D165" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E165" s="7"/>
       <c r="F165" s="12" t="s">
@@ -5157,13 +5157,13 @@
         <v>44</v>
       </c>
       <c r="B166" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C166" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D166" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E166" s="7"/>
       <c r="F166" s="12" t="s">
@@ -5178,13 +5178,13 @@
         <v>44</v>
       </c>
       <c r="B167" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C167" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D167" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E167" s="7"/>
       <c r="F167" s="12" t="s">
@@ -5199,13 +5199,13 @@
         <v>44</v>
       </c>
       <c r="B168" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C168" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D168" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E168" s="7"/>
       <c r="F168" s="12" t="s">
@@ -5220,13 +5220,13 @@
         <v>44</v>
       </c>
       <c r="B169" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C169" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D169" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E169" s="7"/>
       <c r="F169" s="12" t="s">
@@ -5241,13 +5241,13 @@
         <v>44</v>
       </c>
       <c r="B170" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C170" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D170" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E170" s="7"/>
       <c r="F170" s="12" t="s">
@@ -5262,13 +5262,13 @@
         <v>44</v>
       </c>
       <c r="B171" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C171" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D171" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E171" s="7"/>
       <c r="F171" s="12" t="s">
@@ -5283,13 +5283,13 @@
         <v>44</v>
       </c>
       <c r="B172" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C172" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D172" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E172" s="7"/>
       <c r="F172" s="12" t="s">
@@ -5304,13 +5304,13 @@
         <v>44</v>
       </c>
       <c r="B173" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C173" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D173" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E173" s="7"/>
       <c r="F173" s="12" t="s">
@@ -5325,13 +5325,13 @@
         <v>44</v>
       </c>
       <c r="B174" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C174" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D174" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E174" s="7"/>
       <c r="F174" s="12" t="s">
@@ -5346,13 +5346,13 @@
         <v>44</v>
       </c>
       <c r="B175" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C175" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D175" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E175" s="7"/>
       <c r="F175" s="12" t="s">
@@ -5367,13 +5367,13 @@
         <v>44</v>
       </c>
       <c r="B176" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C176" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D176" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E176" s="7"/>
       <c r="F176" s="12" t="s">
@@ -5388,13 +5388,13 @@
         <v>44</v>
       </c>
       <c r="B177" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C177" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D177" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E177" s="7"/>
       <c r="F177" s="12" t="s">
@@ -5409,13 +5409,13 @@
         <v>44</v>
       </c>
       <c r="B178" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C178" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D178" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E178" s="7"/>
       <c r="F178" s="12" t="s">
@@ -5430,13 +5430,13 @@
         <v>44</v>
       </c>
       <c r="B179" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C179" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D179" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E179" s="7"/>
       <c r="F179" s="12" t="s">
@@ -5451,13 +5451,13 @@
         <v>44</v>
       </c>
       <c r="B180" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C180" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D180" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E180" s="7"/>
       <c r="F180" s="12" t="s">
@@ -5472,13 +5472,13 @@
         <v>44</v>
       </c>
       <c r="B181" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C181" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D181" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E181" s="7"/>
       <c r="F181" s="12" t="s">
@@ -5493,13 +5493,13 @@
         <v>44</v>
       </c>
       <c r="B182" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C182" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D182" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E182" s="7"/>
       <c r="F182" s="12" t="s">
@@ -5514,13 +5514,13 @@
         <v>44</v>
       </c>
       <c r="B183" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C183" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D183" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E183" s="7"/>
       <c r="F183" s="12" t="s">
@@ -5535,13 +5535,13 @@
         <v>44</v>
       </c>
       <c r="B184" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C184" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D184" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E184" s="7"/>
       <c r="F184" s="12" t="s">
@@ -5556,13 +5556,13 @@
         <v>44</v>
       </c>
       <c r="B185" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C185" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D185" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E185" s="7"/>
       <c r="F185" s="12" t="s">
@@ -5577,13 +5577,13 @@
         <v>44</v>
       </c>
       <c r="B186" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C186" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D186" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E186" s="7"/>
       <c r="F186" s="12" t="s">
@@ -5598,13 +5598,13 @@
         <v>44</v>
       </c>
       <c r="B187" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C187" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D187" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E187" s="7"/>
       <c r="F187" s="12" t="s">
@@ -5619,13 +5619,13 @@
         <v>44</v>
       </c>
       <c r="B188" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C188" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D188" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E188" s="7"/>
       <c r="F188" s="12" t="s">
@@ -5640,13 +5640,13 @@
         <v>44</v>
       </c>
       <c r="B189" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C189" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D189" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E189" s="7"/>
       <c r="F189" s="12" t="s">
@@ -6860,16 +6860,16 @@
     </row>
     <row r="258" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B258" s="7">
         <v>101</v>
       </c>
       <c r="C258" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D258" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E258" s="7"/>
       <c r="F258" s="12" t="s">
@@ -6881,16 +6881,16 @@
     </row>
     <row r="259" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B259" s="7">
         <v>102</v>
       </c>
       <c r="C259" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D259" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E259" s="7"/>
       <c r="F259" s="12" t="s">
@@ -6902,16 +6902,16 @@
     </row>
     <row r="260" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B260" s="7">
         <v>103</v>
       </c>
       <c r="C260" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D260" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E260" s="7"/>
       <c r="F260" s="12" t="s">
@@ -6923,16 +6923,16 @@
     </row>
     <row r="261" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B261" s="7">
         <v>104</v>
       </c>
       <c r="C261" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D261" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E261" s="7"/>
       <c r="F261" s="12" t="s">
@@ -6944,16 +6944,16 @@
     </row>
     <row r="262" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B262" s="7">
         <v>105</v>
       </c>
       <c r="C262" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D262" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E262" s="7"/>
       <c r="F262" s="12" t="s">
@@ -6965,16 +6965,16 @@
     </row>
     <row r="263" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B263" s="7">
         <v>106</v>
       </c>
       <c r="C263" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D263" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E263" s="7"/>
       <c r="F263" s="12" t="s">
@@ -6986,16 +6986,16 @@
     </row>
     <row r="264" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B264" s="7">
         <v>107</v>
       </c>
       <c r="C264" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D264" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E264" s="7"/>
       <c r="F264" s="12" t="s">
@@ -7007,16 +7007,16 @@
     </row>
     <row r="265" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B265" s="7">
         <v>108</v>
       </c>
       <c r="C265" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D265" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E265" s="7"/>
       <c r="F265" s="12" t="s">
@@ -7028,16 +7028,16 @@
     </row>
     <row r="266" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B266" s="7">
         <v>109</v>
       </c>
       <c r="C266" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D266" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E266" s="7"/>
       <c r="F266" s="12" t="s">
@@ -7049,16 +7049,16 @@
     </row>
     <row r="267" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B267" s="7">
         <v>110</v>
       </c>
       <c r="C267" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D267" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E267" s="7"/>
       <c r="F267" s="12" t="s">
@@ -7070,16 +7070,16 @@
     </row>
     <row r="268" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B268" s="7">
         <v>111</v>
       </c>
       <c r="C268" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D268" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E268" s="7"/>
       <c r="F268" s="12" t="s">
@@ -7091,16 +7091,16 @@
     </row>
     <row r="269" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B269" s="7">
         <v>112</v>
       </c>
       <c r="C269" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D269" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E269" s="7"/>
       <c r="F269" s="12" t="s">
@@ -7112,16 +7112,16 @@
     </row>
     <row r="270" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B270" s="7">
         <v>113</v>
       </c>
       <c r="C270" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D270" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E270" s="7"/>
       <c r="F270" s="12" t="s">
@@ -7133,16 +7133,16 @@
     </row>
     <row r="271" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B271" s="7">
         <v>114</v>
       </c>
       <c r="C271" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D271" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E271" s="7"/>
       <c r="F271" s="12" t="s">
@@ -7154,16 +7154,16 @@
     </row>
     <row r="272" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B272" s="7">
         <v>115</v>
       </c>
       <c r="C272" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D272" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E272" s="7"/>
       <c r="F272" s="12" t="s">
@@ -7175,16 +7175,16 @@
     </row>
     <row r="273" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B273" s="7">
         <v>116</v>
       </c>
       <c r="C273" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D273" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E273" s="7"/>
       <c r="F273" s="12" t="s">
@@ -7196,16 +7196,16 @@
     </row>
     <row r="274" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B274" s="7">
         <v>117</v>
       </c>
       <c r="C274" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D274" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E274" s="7"/>
       <c r="F274" s="12" t="s">
@@ -7217,16 +7217,16 @@
     </row>
     <row r="275" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B275" s="7">
         <v>118</v>
       </c>
       <c r="C275" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D275" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E275" s="7"/>
       <c r="F275" s="12" t="s">
@@ -7238,16 +7238,16 @@
     </row>
     <row r="276" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B276" s="7">
         <v>119</v>
       </c>
       <c r="C276" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D276" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E276" s="7"/>
       <c r="F276" s="12" t="s">
@@ -7259,16 +7259,16 @@
     </row>
     <row r="277" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B277" s="7">
         <v>120</v>
       </c>
       <c r="C277" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D277" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E277" s="7"/>
       <c r="F277" s="12" t="s">
@@ -7280,16 +7280,16 @@
     </row>
     <row r="278" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B278" s="7">
         <v>121</v>
       </c>
       <c r="C278" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D278" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E278" s="7"/>
       <c r="F278" s="12" t="s">
@@ -7301,16 +7301,16 @@
     </row>
     <row r="279" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B279" s="7">
         <v>122</v>
       </c>
       <c r="C279" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D279" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E279" s="7"/>
       <c r="F279" s="12" t="s">
@@ -7322,16 +7322,16 @@
     </row>
     <row r="280" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B280" s="7">
         <v>123</v>
       </c>
       <c r="C280" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D280" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E280" s="7"/>
       <c r="F280" s="12" t="s">
@@ -7343,16 +7343,16 @@
     </row>
     <row r="281" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B281" s="7">
         <v>124</v>
       </c>
       <c r="C281" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D281" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E281" s="7"/>
       <c r="F281" s="12" t="s">
@@ -7364,16 +7364,16 @@
     </row>
     <row r="282" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B282" s="7">
         <v>125</v>
       </c>
       <c r="C282" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D282" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E282" s="7"/>
       <c r="F282" s="12" t="s">
@@ -7385,16 +7385,16 @@
     </row>
     <row r="283" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B283" s="7">
         <v>126</v>
       </c>
       <c r="C283" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D283" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E283" s="7"/>
       <c r="F283" s="12" t="s">
@@ -7406,16 +7406,16 @@
     </row>
     <row r="284" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B284" s="7">
         <v>127</v>
       </c>
       <c r="C284" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D284" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E284" s="7"/>
       <c r="F284" s="12" t="s">
@@ -7427,16 +7427,16 @@
     </row>
     <row r="285" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B285" s="7">
         <v>128</v>
       </c>
       <c r="C285" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D285" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E285" s="7"/>
       <c r="F285" s="12" t="s">
@@ -7448,16 +7448,16 @@
     </row>
     <row r="286" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B286" s="7">
         <v>129</v>
       </c>
       <c r="C286" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D286" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E286" s="7"/>
       <c r="F286" s="12" t="s">
@@ -7469,16 +7469,16 @@
     </row>
     <row r="287" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B287" s="7">
         <v>130</v>
       </c>
       <c r="C287" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D287" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E287" s="7"/>
       <c r="F287" s="12" t="s">
@@ -7490,16 +7490,16 @@
     </row>
     <row r="288" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B288" s="7">
         <v>131</v>
       </c>
       <c r="C288" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D288" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E288" s="7"/>
       <c r="F288" s="12" t="s">
@@ -7511,16 +7511,16 @@
     </row>
     <row r="289" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B289" s="7">
         <v>132</v>
       </c>
       <c r="C289" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D289" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E289" s="7"/>
       <c r="F289" s="12" t="s">
@@ -7532,16 +7532,16 @@
     </row>
     <row r="290" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B290" s="7">
         <v>133</v>
       </c>
       <c r="C290" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D290" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E290" s="7"/>
       <c r="F290" s="12" t="s">
@@ -7553,16 +7553,16 @@
     </row>
     <row r="291" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B291" s="7">
         <v>134</v>
       </c>
       <c r="C291" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D291" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E291" s="7"/>
       <c r="F291" s="12" t="s">
@@ -7574,16 +7574,16 @@
     </row>
     <row r="292" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B292" s="7">
         <v>135</v>
       </c>
       <c r="C292" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D292" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E292" s="7"/>
       <c r="F292" s="12" t="s">
@@ -7595,16 +7595,16 @@
     </row>
     <row r="293" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B293" s="7">
         <v>136</v>
       </c>
       <c r="C293" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D293" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E293" s="7"/>
       <c r="F293" s="12" t="s">
@@ -7616,16 +7616,16 @@
     </row>
     <row r="294" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B294" s="7">
         <v>137</v>
       </c>
       <c r="C294" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D294" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E294" s="7"/>
       <c r="F294" s="12" t="s">
@@ -7637,16 +7637,16 @@
     </row>
     <row r="295" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B295" s="7">
         <v>138</v>
       </c>
       <c r="C295" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D295" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E295" s="7"/>
       <c r="F295" s="12" t="s">
@@ -7658,16 +7658,16 @@
     </row>
     <row r="296" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B296" s="7">
         <v>139</v>
       </c>
       <c r="C296" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D296" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E296" s="7"/>
       <c r="F296" s="12" t="s">
@@ -7679,16 +7679,16 @@
     </row>
     <row r="297" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B297" s="7">
         <v>140</v>
       </c>
       <c r="C297" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D297" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E297" s="7"/>
       <c r="F297" s="12" t="s">
@@ -7700,16 +7700,16 @@
     </row>
     <row r="298" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B298" s="7">
         <v>141</v>
       </c>
       <c r="C298" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D298" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E298" s="7"/>
       <c r="F298" s="12" t="s">
@@ -7721,16 +7721,16 @@
     </row>
     <row r="299" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B299" s="7">
         <v>142</v>
       </c>
       <c r="C299" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D299" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E299" s="7"/>
       <c r="F299" s="12" t="s">
@@ -7742,16 +7742,16 @@
     </row>
     <row r="300" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B300" s="7">
         <v>143</v>
       </c>
       <c r="C300" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D300" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E300" s="7"/>
       <c r="F300" s="12" t="s">
@@ -7763,16 +7763,16 @@
     </row>
     <row r="301" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B301" s="7">
         <v>144</v>
       </c>
       <c r="C301" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D301" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E301" s="7"/>
       <c r="F301" s="12" t="s">
@@ -7784,16 +7784,16 @@
     </row>
     <row r="302" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B302" s="7">
         <v>145</v>
       </c>
       <c r="C302" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D302" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E302" s="7"/>
       <c r="F302" s="12" t="s">
@@ -7805,16 +7805,16 @@
     </row>
     <row r="303" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B303" s="7">
         <v>146</v>
       </c>
       <c r="C303" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D303" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E303" s="7"/>
       <c r="F303" s="12" t="s">
@@ -7826,16 +7826,16 @@
     </row>
     <row r="304" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B304" s="7">
         <v>147</v>
       </c>
       <c r="C304" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D304" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E304" s="7"/>
       <c r="F304" s="12" t="s">
@@ -7847,16 +7847,16 @@
     </row>
     <row r="305" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B305" s="7">
         <v>148</v>
       </c>
       <c r="C305" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D305" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E305" s="7"/>
       <c r="F305" s="12" t="s">
@@ -7868,16 +7868,16 @@
     </row>
     <row r="306" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B306" s="7">
         <v>149</v>
       </c>
       <c r="C306" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D306" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E306" s="7"/>
       <c r="F306" s="12" t="s">
@@ -7889,16 +7889,16 @@
     </row>
     <row r="307" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B307" s="7">
         <v>150</v>
       </c>
       <c r="C307" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D307" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E307" s="7"/>
       <c r="F307" s="12" t="s">
@@ -7910,16 +7910,16 @@
     </row>
     <row r="308" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B308" s="7">
         <v>151</v>
       </c>
       <c r="C308" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D308" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E308" s="7"/>
       <c r="F308" s="12" t="s">
@@ -7931,16 +7931,16 @@
     </row>
     <row r="309" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B309" s="7">
         <v>152</v>
       </c>
       <c r="C309" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D309" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E309" s="7"/>
       <c r="F309" s="12" t="s">
@@ -7952,16 +7952,16 @@
     </row>
     <row r="310" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B310" s="7">
         <v>153</v>
       </c>
       <c r="C310" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D310" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E310" s="7"/>
       <c r="F310" s="12" t="s">
@@ -7973,16 +7973,16 @@
     </row>
     <row r="311" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B311" s="7">
         <v>154</v>
       </c>
       <c r="C311" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D311" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E311" s="7"/>
       <c r="F311" s="12" t="s">
@@ -7994,16 +7994,16 @@
     </row>
     <row r="312" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B312" s="7">
         <v>155</v>
       </c>
       <c r="C312" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D312" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E312" s="7"/>
       <c r="F312" s="12" t="s">
@@ -8015,16 +8015,16 @@
     </row>
     <row r="313" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B313" s="7">
         <v>156</v>
       </c>
       <c r="C313" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D313" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E313" s="7"/>
       <c r="F313" s="12" t="s">
@@ -8036,16 +8036,16 @@
     </row>
     <row r="314" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B314" s="7">
         <v>157</v>
       </c>
       <c r="C314" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D314" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E314" s="7"/>
       <c r="F314" s="12" t="s">
@@ -8057,16 +8057,16 @@
     </row>
     <row r="315" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B315" s="7">
         <v>158</v>
       </c>
       <c r="C315" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D315" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E315" s="7"/>
       <c r="F315" s="12" t="s">
@@ -8078,16 +8078,16 @@
     </row>
     <row r="316" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B316" s="7">
         <v>159</v>
       </c>
       <c r="C316" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D316" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E316" s="7"/>
       <c r="F316" s="12" t="s">
@@ -8099,16 +8099,16 @@
     </row>
     <row r="317" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B317" s="7">
         <v>160</v>
       </c>
       <c r="C317" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D317" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E317" s="7"/>
       <c r="F317" s="12" t="s">
@@ -8120,16 +8120,16 @@
     </row>
     <row r="318" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B318" s="7">
         <v>161</v>
       </c>
       <c r="C318" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D318" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E318" s="7"/>
       <c r="F318" s="12" t="s">
@@ -8141,16 +8141,16 @@
     </row>
     <row r="319" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B319" s="7">
         <v>162</v>
       </c>
       <c r="C319" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D319" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E319" s="7"/>
       <c r="F319" s="12" t="s">
@@ -8162,16 +8162,16 @@
     </row>
     <row r="320" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B320" s="7">
         <v>163</v>
       </c>
       <c r="C320" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D320" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E320" s="7"/>
       <c r="F320" s="12" t="s">
@@ -8183,16 +8183,16 @@
     </row>
     <row r="321" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B321" s="7">
         <v>164</v>
       </c>
       <c r="C321" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D321" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E321" s="7"/>
       <c r="F321" s="12" t="s">
@@ -8204,16 +8204,16 @@
     </row>
     <row r="322" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B322" s="7">
         <v>165</v>
       </c>
       <c r="C322" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D322" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E322" s="7"/>
       <c r="F322" s="12" t="s">
@@ -8225,16 +8225,16 @@
     </row>
     <row r="323" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B323" s="7">
         <v>166</v>
       </c>
       <c r="C323" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D323" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E323" s="7"/>
       <c r="F323" s="12" t="s">
@@ -8257,8 +8257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8282,12 +8282,12 @@
         <v>14</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>216</v>
+        <v>307</v>
       </c>
       <c r="B2" t="s">
         <v>215</v>
@@ -8324,16 +8324,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CI: Pre-TAS may 2021 - some improvements.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/May 2021/ci_lf_pretas_1_site_202105.xlsx
+++ b/LF/PreTAS/Ivory Coast/May 2021/ci_lf_pretas_1_site_202105.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\May 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2CD5DB-9382-45A5-8FB8-9872889EDAA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F137450-5462-4A60-AD67-278444480F05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,9 +678,6 @@
     <t>site_list = ${c_site}</t>
   </si>
   <si>
-    <t>ci_lf_pretas_1_site_202105_v2</t>
-  </si>
-  <si>
     <t>Autre</t>
   </si>
   <si>
@@ -954,7 +951,10 @@
     <t>Type Dest</t>
   </si>
   <si>
-    <t>(May 2021) 1. Côte d'Ivoire - Pre TAS FL Fromulaire Site V2</t>
+    <t>(May 2021) 1. Côte d'Ivoire - Pre TAS FL Fromulaire Site V3</t>
+  </si>
+  <si>
+    <t>ci_lf_pretas_1_site_202105_v3</t>
   </si>
 </sst>
 </file>
@@ -1627,11 +1627,11 @@
         <v>205</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="8"/>
@@ -1639,7 +1639,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="4" t="s">
@@ -1656,22 +1656,22 @@
         <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>289</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" t="s">
         <v>284</v>
       </c>
-      <c r="F9" t="s">
-        <v>285</v>
-      </c>
       <c r="K9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M9" t="s">
         <v>56</v>
@@ -1679,25 +1679,25 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" t="s">
+        <v>299</v>
+      </c>
+      <c r="E10" t="s">
         <v>290</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
+        <v>285</v>
+      </c>
+      <c r="K10" t="s">
         <v>300</v>
-      </c>
-      <c r="E10" t="s">
-        <v>291</v>
-      </c>
-      <c r="F10" t="s">
-        <v>286</v>
-      </c>
-      <c r="K10" t="s">
-        <v>301</v>
       </c>
       <c r="M10" t="s">
         <v>56</v>
@@ -1795,14 +1795,14 @@
         <v>45</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -4275,13 +4275,13 @@
         <v>44</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="12" t="s">
@@ -4296,13 +4296,13 @@
         <v>44</v>
       </c>
       <c r="B125" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C125" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D125" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E125" s="7"/>
       <c r="F125" s="12" t="s">
@@ -4317,13 +4317,13 @@
         <v>44</v>
       </c>
       <c r="B126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E126" s="7"/>
       <c r="F126" s="12" t="s">
@@ -4338,13 +4338,13 @@
         <v>44</v>
       </c>
       <c r="B127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E127" s="7"/>
       <c r="F127" s="12" t="s">
@@ -4359,13 +4359,13 @@
         <v>44</v>
       </c>
       <c r="B128" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C128" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D128" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="12" t="s">
@@ -4380,13 +4380,13 @@
         <v>44</v>
       </c>
       <c r="B129" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C129" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D129" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E129" s="7"/>
       <c r="F129" s="12" t="s">
@@ -4401,13 +4401,13 @@
         <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C130" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D130" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E130" s="7"/>
       <c r="F130" s="12" t="s">
@@ -4422,13 +4422,13 @@
         <v>44</v>
       </c>
       <c r="B131" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C131" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D131" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E131" s="7"/>
       <c r="F131" s="12" t="s">
@@ -4443,13 +4443,13 @@
         <v>44</v>
       </c>
       <c r="B132" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C132" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D132" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E132" s="7"/>
       <c r="F132" s="12" t="s">
@@ -4464,13 +4464,13 @@
         <v>44</v>
       </c>
       <c r="B133" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C133" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D133" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E133" s="7"/>
       <c r="F133" s="12" t="s">
@@ -4485,13 +4485,13 @@
         <v>44</v>
       </c>
       <c r="B134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E134" s="7"/>
       <c r="F134" s="12" t="s">
@@ -4506,13 +4506,13 @@
         <v>44</v>
       </c>
       <c r="B135" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D135" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E135" s="7"/>
       <c r="F135" s="12" t="s">
@@ -4527,13 +4527,13 @@
         <v>44</v>
       </c>
       <c r="B136" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C136" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D136" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E136" s="7"/>
       <c r="F136" s="12" t="s">
@@ -4548,13 +4548,13 @@
         <v>44</v>
       </c>
       <c r="B137" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C137" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D137" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="12" t="s">
@@ -4569,13 +4569,13 @@
         <v>44</v>
       </c>
       <c r="B138" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C138" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D138" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E138" s="7"/>
       <c r="F138" s="12" t="s">
@@ -4590,13 +4590,13 @@
         <v>44</v>
       </c>
       <c r="B139" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C139" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D139" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" s="12" t="s">
@@ -4611,13 +4611,13 @@
         <v>44</v>
       </c>
       <c r="B140" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C140" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D140" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E140" s="7"/>
       <c r="F140" s="12" t="s">
@@ -4632,13 +4632,13 @@
         <v>44</v>
       </c>
       <c r="B141" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C141" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D141" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="12" t="s">
@@ -4653,13 +4653,13 @@
         <v>44</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C142" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D142" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E142" s="7"/>
       <c r="F142" s="12" t="s">
@@ -4674,13 +4674,13 @@
         <v>44</v>
       </c>
       <c r="B143" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C143" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D143" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E143" s="7"/>
       <c r="F143" s="12" t="s">
@@ -4695,13 +4695,13 @@
         <v>44</v>
       </c>
       <c r="B144" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C144" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D144" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E144" s="7"/>
       <c r="F144" s="12" t="s">
@@ -4716,13 +4716,13 @@
         <v>44</v>
       </c>
       <c r="B145" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C145" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D145" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="12" t="s">
@@ -4737,13 +4737,13 @@
         <v>44</v>
       </c>
       <c r="B146" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C146" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D146" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E146" s="7"/>
       <c r="F146" s="12" t="s">
@@ -4758,13 +4758,13 @@
         <v>44</v>
       </c>
       <c r="B147" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C147" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D147" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E147" s="7"/>
       <c r="F147" s="12" t="s">
@@ -4779,13 +4779,13 @@
         <v>44</v>
       </c>
       <c r="B148" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C148" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D148" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E148" s="7"/>
       <c r="F148" s="12" t="s">
@@ -4800,13 +4800,13 @@
         <v>44</v>
       </c>
       <c r="B149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E149" s="7"/>
       <c r="F149" s="12" t="s">
@@ -4821,13 +4821,13 @@
         <v>44</v>
       </c>
       <c r="B150" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C150" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D150" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E150" s="7"/>
       <c r="F150" s="12" t="s">
@@ -4842,13 +4842,13 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C151" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D151" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E151" s="7"/>
       <c r="F151" s="12" t="s">
@@ -4863,13 +4863,13 @@
         <v>44</v>
       </c>
       <c r="B152" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C152" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D152" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E152" s="7"/>
       <c r="F152" s="12" t="s">
@@ -4884,13 +4884,13 @@
         <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E153" s="7"/>
       <c r="F153" s="12" t="s">
@@ -4905,13 +4905,13 @@
         <v>44</v>
       </c>
       <c r="B154" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C154" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D154" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E154" s="7"/>
       <c r="F154" s="12" t="s">
@@ -4926,13 +4926,13 @@
         <v>44</v>
       </c>
       <c r="B155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E155" s="7"/>
       <c r="F155" s="12" t="s">
@@ -4947,13 +4947,13 @@
         <v>44</v>
       </c>
       <c r="B156" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C156" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D156" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E156" s="7"/>
       <c r="F156" s="12" t="s">
@@ -4968,13 +4968,13 @@
         <v>44</v>
       </c>
       <c r="B157" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C157" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D157" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E157" s="7"/>
       <c r="F157" s="12" t="s">
@@ -4989,13 +4989,13 @@
         <v>44</v>
       </c>
       <c r="B158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E158" s="7"/>
       <c r="F158" s="12" t="s">
@@ -5010,13 +5010,13 @@
         <v>44</v>
       </c>
       <c r="B159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E159" s="7"/>
       <c r="F159" s="12" t="s">
@@ -5031,13 +5031,13 @@
         <v>44</v>
       </c>
       <c r="B160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E160" s="7"/>
       <c r="F160" s="12" t="s">
@@ -5052,13 +5052,13 @@
         <v>44</v>
       </c>
       <c r="B161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E161" s="7"/>
       <c r="F161" s="12" t="s">
@@ -5073,13 +5073,13 @@
         <v>44</v>
       </c>
       <c r="B162" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C162" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D162" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E162" s="7"/>
       <c r="F162" s="12" t="s">
@@ -5094,13 +5094,13 @@
         <v>44</v>
       </c>
       <c r="B163" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C163" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D163" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E163" s="7"/>
       <c r="F163" s="12" t="s">
@@ -5115,13 +5115,13 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C164" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D164" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E164" s="7"/>
       <c r="F164" s="12" t="s">
@@ -5136,13 +5136,13 @@
         <v>44</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C165" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D165" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E165" s="7"/>
       <c r="F165" s="12" t="s">
@@ -5157,13 +5157,13 @@
         <v>44</v>
       </c>
       <c r="B166" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C166" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D166" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E166" s="7"/>
       <c r="F166" s="12" t="s">
@@ -5178,13 +5178,13 @@
         <v>44</v>
       </c>
       <c r="B167" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C167" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D167" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E167" s="7"/>
       <c r="F167" s="12" t="s">
@@ -5199,13 +5199,13 @@
         <v>44</v>
       </c>
       <c r="B168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E168" s="7"/>
       <c r="F168" s="12" t="s">
@@ -5220,13 +5220,13 @@
         <v>44</v>
       </c>
       <c r="B169" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C169" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D169" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E169" s="7"/>
       <c r="F169" s="12" t="s">
@@ -5241,13 +5241,13 @@
         <v>44</v>
       </c>
       <c r="B170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E170" s="7"/>
       <c r="F170" s="12" t="s">
@@ -5262,13 +5262,13 @@
         <v>44</v>
       </c>
       <c r="B171" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C171" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D171" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E171" s="7"/>
       <c r="F171" s="12" t="s">
@@ -5283,13 +5283,13 @@
         <v>44</v>
       </c>
       <c r="B172" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C172" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D172" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E172" s="7"/>
       <c r="F172" s="12" t="s">
@@ -5304,13 +5304,13 @@
         <v>44</v>
       </c>
       <c r="B173" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C173" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D173" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E173" s="7"/>
       <c r="F173" s="12" t="s">
@@ -5325,13 +5325,13 @@
         <v>44</v>
       </c>
       <c r="B174" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C174" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D174" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E174" s="7"/>
       <c r="F174" s="12" t="s">
@@ -5346,13 +5346,13 @@
         <v>44</v>
       </c>
       <c r="B175" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C175" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D175" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E175" s="7"/>
       <c r="F175" s="12" t="s">
@@ -5367,13 +5367,13 @@
         <v>44</v>
       </c>
       <c r="B176" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C176" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D176" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E176" s="7"/>
       <c r="F176" s="12" t="s">
@@ -5388,13 +5388,13 @@
         <v>44</v>
       </c>
       <c r="B177" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C177" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D177" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E177" s="7"/>
       <c r="F177" s="12" t="s">
@@ -5409,13 +5409,13 @@
         <v>44</v>
       </c>
       <c r="B178" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C178" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D178" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E178" s="7"/>
       <c r="F178" s="12" t="s">
@@ -5430,13 +5430,13 @@
         <v>44</v>
       </c>
       <c r="B179" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C179" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D179" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E179" s="7"/>
       <c r="F179" s="12" t="s">
@@ -5451,13 +5451,13 @@
         <v>44</v>
       </c>
       <c r="B180" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C180" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D180" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E180" s="7"/>
       <c r="F180" s="12" t="s">
@@ -5472,13 +5472,13 @@
         <v>44</v>
       </c>
       <c r="B181" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C181" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D181" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E181" s="7"/>
       <c r="F181" s="12" t="s">
@@ -5493,13 +5493,13 @@
         <v>44</v>
       </c>
       <c r="B182" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C182" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D182" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E182" s="7"/>
       <c r="F182" s="12" t="s">
@@ -5514,13 +5514,13 @@
         <v>44</v>
       </c>
       <c r="B183" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C183" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D183" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E183" s="7"/>
       <c r="F183" s="12" t="s">
@@ -5535,13 +5535,13 @@
         <v>44</v>
       </c>
       <c r="B184" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C184" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D184" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E184" s="7"/>
       <c r="F184" s="12" t="s">
@@ -5556,13 +5556,13 @@
         <v>44</v>
       </c>
       <c r="B185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E185" s="7"/>
       <c r="F185" s="12" t="s">
@@ -5577,13 +5577,13 @@
         <v>44</v>
       </c>
       <c r="B186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E186" s="7"/>
       <c r="F186" s="12" t="s">
@@ -5598,13 +5598,13 @@
         <v>44</v>
       </c>
       <c r="B187" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C187" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D187" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E187" s="7"/>
       <c r="F187" s="12" t="s">
@@ -5619,13 +5619,13 @@
         <v>44</v>
       </c>
       <c r="B188" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C188" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D188" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E188" s="7"/>
       <c r="F188" s="12" t="s">
@@ -5640,13 +5640,13 @@
         <v>44</v>
       </c>
       <c r="B189" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C189" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D189" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E189" s="7"/>
       <c r="F189" s="12" t="s">
@@ -6860,16 +6860,16 @@
     </row>
     <row r="258" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B258" s="7">
         <v>101</v>
       </c>
       <c r="C258" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D258" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E258" s="7"/>
       <c r="F258" s="12" t="s">
@@ -6881,16 +6881,16 @@
     </row>
     <row r="259" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B259" s="7">
         <v>102</v>
       </c>
       <c r="C259" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D259" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E259" s="7"/>
       <c r="F259" s="12" t="s">
@@ -6902,16 +6902,16 @@
     </row>
     <row r="260" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B260" s="7">
         <v>103</v>
       </c>
       <c r="C260" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D260" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E260" s="7"/>
       <c r="F260" s="12" t="s">
@@ -6923,16 +6923,16 @@
     </row>
     <row r="261" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B261" s="7">
         <v>104</v>
       </c>
       <c r="C261" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D261" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E261" s="7"/>
       <c r="F261" s="12" t="s">
@@ -6944,16 +6944,16 @@
     </row>
     <row r="262" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B262" s="7">
         <v>105</v>
       </c>
       <c r="C262" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D262" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E262" s="7"/>
       <c r="F262" s="12" t="s">
@@ -6965,16 +6965,16 @@
     </row>
     <row r="263" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B263" s="7">
         <v>106</v>
       </c>
       <c r="C263" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D263" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E263" s="7"/>
       <c r="F263" s="12" t="s">
@@ -6986,16 +6986,16 @@
     </row>
     <row r="264" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B264" s="7">
         <v>107</v>
       </c>
       <c r="C264" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D264" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E264" s="7"/>
       <c r="F264" s="12" t="s">
@@ -7007,16 +7007,16 @@
     </row>
     <row r="265" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B265" s="7">
         <v>108</v>
       </c>
       <c r="C265" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D265" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E265" s="7"/>
       <c r="F265" s="12" t="s">
@@ -7028,16 +7028,16 @@
     </row>
     <row r="266" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B266" s="7">
         <v>109</v>
       </c>
       <c r="C266" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D266" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E266" s="7"/>
       <c r="F266" s="12" t="s">
@@ -7049,16 +7049,16 @@
     </row>
     <row r="267" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B267" s="7">
         <v>110</v>
       </c>
       <c r="C267" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D267" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E267" s="7"/>
       <c r="F267" s="12" t="s">
@@ -7070,16 +7070,16 @@
     </row>
     <row r="268" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B268" s="7">
         <v>111</v>
       </c>
       <c r="C268" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D268" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E268" s="7"/>
       <c r="F268" s="12" t="s">
@@ -7091,16 +7091,16 @@
     </row>
     <row r="269" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B269" s="7">
         <v>112</v>
       </c>
       <c r="C269" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D269" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E269" s="7"/>
       <c r="F269" s="12" t="s">
@@ -7112,16 +7112,16 @@
     </row>
     <row r="270" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B270" s="7">
         <v>113</v>
       </c>
       <c r="C270" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D270" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E270" s="7"/>
       <c r="F270" s="12" t="s">
@@ -7133,16 +7133,16 @@
     </row>
     <row r="271" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B271" s="7">
         <v>114</v>
       </c>
       <c r="C271" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D271" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E271" s="7"/>
       <c r="F271" s="12" t="s">
@@ -7154,16 +7154,16 @@
     </row>
     <row r="272" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B272" s="7">
         <v>115</v>
       </c>
       <c r="C272" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D272" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E272" s="7"/>
       <c r="F272" s="12" t="s">
@@ -7175,16 +7175,16 @@
     </row>
     <row r="273" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B273" s="7">
         <v>116</v>
       </c>
       <c r="C273" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D273" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E273" s="7"/>
       <c r="F273" s="12" t="s">
@@ -7196,16 +7196,16 @@
     </row>
     <row r="274" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B274" s="7">
         <v>117</v>
       </c>
       <c r="C274" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D274" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E274" s="7"/>
       <c r="F274" s="12" t="s">
@@ -7217,16 +7217,16 @@
     </row>
     <row r="275" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B275" s="7">
         <v>118</v>
       </c>
       <c r="C275" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D275" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E275" s="7"/>
       <c r="F275" s="12" t="s">
@@ -7238,16 +7238,16 @@
     </row>
     <row r="276" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B276" s="7">
         <v>119</v>
       </c>
       <c r="C276" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D276" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E276" s="7"/>
       <c r="F276" s="12" t="s">
@@ -7259,16 +7259,16 @@
     </row>
     <row r="277" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B277" s="7">
         <v>120</v>
       </c>
       <c r="C277" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D277" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E277" s="7"/>
       <c r="F277" s="12" t="s">
@@ -7280,16 +7280,16 @@
     </row>
     <row r="278" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B278" s="7">
         <v>121</v>
       </c>
       <c r="C278" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D278" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E278" s="7"/>
       <c r="F278" s="12" t="s">
@@ -7301,16 +7301,16 @@
     </row>
     <row r="279" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B279" s="7">
         <v>122</v>
       </c>
       <c r="C279" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D279" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E279" s="7"/>
       <c r="F279" s="12" t="s">
@@ -7322,16 +7322,16 @@
     </row>
     <row r="280" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B280" s="7">
         <v>123</v>
       </c>
       <c r="C280" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D280" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E280" s="7"/>
       <c r="F280" s="12" t="s">
@@ -7343,16 +7343,16 @@
     </row>
     <row r="281" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B281" s="7">
         <v>124</v>
       </c>
       <c r="C281" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D281" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E281" s="7"/>
       <c r="F281" s="12" t="s">
@@ -7364,16 +7364,16 @@
     </row>
     <row r="282" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B282" s="7">
         <v>125</v>
       </c>
       <c r="C282" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D282" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E282" s="7"/>
       <c r="F282" s="12" t="s">
@@ -7385,16 +7385,16 @@
     </row>
     <row r="283" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B283" s="7">
         <v>126</v>
       </c>
       <c r="C283" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D283" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E283" s="7"/>
       <c r="F283" s="12" t="s">
@@ -7406,16 +7406,16 @@
     </row>
     <row r="284" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B284" s="7">
         <v>127</v>
       </c>
       <c r="C284" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D284" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E284" s="7"/>
       <c r="F284" s="12" t="s">
@@ -7427,16 +7427,16 @@
     </row>
     <row r="285" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B285" s="7">
         <v>128</v>
       </c>
       <c r="C285" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D285" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E285" s="7"/>
       <c r="F285" s="12" t="s">
@@ -7448,16 +7448,16 @@
     </row>
     <row r="286" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B286" s="7">
         <v>129</v>
       </c>
       <c r="C286" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D286" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E286" s="7"/>
       <c r="F286" s="12" t="s">
@@ -7469,16 +7469,16 @@
     </row>
     <row r="287" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B287" s="7">
         <v>130</v>
       </c>
       <c r="C287" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D287" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E287" s="7"/>
       <c r="F287" s="12" t="s">
@@ -7490,16 +7490,16 @@
     </row>
     <row r="288" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B288" s="7">
         <v>131</v>
       </c>
       <c r="C288" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D288" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E288" s="7"/>
       <c r="F288" s="12" t="s">
@@ -7511,16 +7511,16 @@
     </row>
     <row r="289" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B289" s="7">
         <v>132</v>
       </c>
       <c r="C289" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D289" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E289" s="7"/>
       <c r="F289" s="12" t="s">
@@ -7532,16 +7532,16 @@
     </row>
     <row r="290" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B290" s="7">
         <v>133</v>
       </c>
       <c r="C290" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D290" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E290" s="7"/>
       <c r="F290" s="12" t="s">
@@ -7553,16 +7553,16 @@
     </row>
     <row r="291" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B291" s="7">
         <v>134</v>
       </c>
       <c r="C291" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D291" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E291" s="7"/>
       <c r="F291" s="12" t="s">
@@ -7574,16 +7574,16 @@
     </row>
     <row r="292" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B292" s="7">
         <v>135</v>
       </c>
       <c r="C292" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D292" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E292" s="7"/>
       <c r="F292" s="12" t="s">
@@ -7595,16 +7595,16 @@
     </row>
     <row r="293" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B293" s="7">
         <v>136</v>
       </c>
       <c r="C293" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D293" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E293" s="7"/>
       <c r="F293" s="12" t="s">
@@ -7616,16 +7616,16 @@
     </row>
     <row r="294" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B294" s="7">
         <v>137</v>
       </c>
       <c r="C294" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D294" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E294" s="7"/>
       <c r="F294" s="12" t="s">
@@ -7637,16 +7637,16 @@
     </row>
     <row r="295" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B295" s="7">
         <v>138</v>
       </c>
       <c r="C295" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D295" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E295" s="7"/>
       <c r="F295" s="12" t="s">
@@ -7658,16 +7658,16 @@
     </row>
     <row r="296" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B296" s="7">
         <v>139</v>
       </c>
       <c r="C296" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D296" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E296" s="7"/>
       <c r="F296" s="12" t="s">
@@ -7679,16 +7679,16 @@
     </row>
     <row r="297" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B297" s="7">
         <v>140</v>
       </c>
       <c r="C297" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D297" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E297" s="7"/>
       <c r="F297" s="12" t="s">
@@ -7700,16 +7700,16 @@
     </row>
     <row r="298" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B298" s="7">
         <v>141</v>
       </c>
       <c r="C298" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D298" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E298" s="7"/>
       <c r="F298" s="12" t="s">
@@ -7721,16 +7721,16 @@
     </row>
     <row r="299" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B299" s="7">
         <v>142</v>
       </c>
       <c r="C299" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D299" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E299" s="7"/>
       <c r="F299" s="12" t="s">
@@ -7742,16 +7742,16 @@
     </row>
     <row r="300" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B300" s="7">
         <v>143</v>
       </c>
       <c r="C300" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D300" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E300" s="7"/>
       <c r="F300" s="12" t="s">
@@ -7763,16 +7763,16 @@
     </row>
     <row r="301" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B301" s="7">
         <v>144</v>
       </c>
       <c r="C301" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D301" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E301" s="7"/>
       <c r="F301" s="12" t="s">
@@ -7784,16 +7784,16 @@
     </row>
     <row r="302" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B302" s="7">
         <v>145</v>
       </c>
       <c r="C302" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D302" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E302" s="7"/>
       <c r="F302" s="12" t="s">
@@ -7805,16 +7805,16 @@
     </row>
     <row r="303" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B303" s="7">
         <v>146</v>
       </c>
       <c r="C303" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D303" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E303" s="7"/>
       <c r="F303" s="12" t="s">
@@ -7826,16 +7826,16 @@
     </row>
     <row r="304" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B304" s="7">
         <v>147</v>
       </c>
       <c r="C304" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D304" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E304" s="7"/>
       <c r="F304" s="12" t="s">
@@ -7847,16 +7847,16 @@
     </row>
     <row r="305" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B305" s="7">
         <v>148</v>
       </c>
       <c r="C305" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D305" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E305" s="7"/>
       <c r="F305" s="12" t="s">
@@ -7868,16 +7868,16 @@
     </row>
     <row r="306" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B306" s="7">
         <v>149</v>
       </c>
       <c r="C306" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D306" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E306" s="7"/>
       <c r="F306" s="12" t="s">
@@ -7889,16 +7889,16 @@
     </row>
     <row r="307" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B307" s="7">
         <v>150</v>
       </c>
       <c r="C307" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D307" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E307" s="7"/>
       <c r="F307" s="12" t="s">
@@ -7910,16 +7910,16 @@
     </row>
     <row r="308" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B308" s="7">
         <v>151</v>
       </c>
       <c r="C308" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D308" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E308" s="7"/>
       <c r="F308" s="12" t="s">
@@ -7931,16 +7931,16 @@
     </row>
     <row r="309" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B309" s="7">
         <v>152</v>
       </c>
       <c r="C309" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D309" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E309" s="7"/>
       <c r="F309" s="12" t="s">
@@ -7952,16 +7952,16 @@
     </row>
     <row r="310" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B310" s="7">
         <v>153</v>
       </c>
       <c r="C310" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D310" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E310" s="7"/>
       <c r="F310" s="12" t="s">
@@ -7973,16 +7973,16 @@
     </row>
     <row r="311" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B311" s="7">
         <v>154</v>
       </c>
       <c r="C311" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D311" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E311" s="7"/>
       <c r="F311" s="12" t="s">
@@ -7994,16 +7994,16 @@
     </row>
     <row r="312" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B312" s="7">
         <v>155</v>
       </c>
       <c r="C312" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D312" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E312" s="7"/>
       <c r="F312" s="12" t="s">
@@ -8015,16 +8015,16 @@
     </row>
     <row r="313" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B313" s="7">
         <v>156</v>
       </c>
       <c r="C313" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D313" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E313" s="7"/>
       <c r="F313" s="12" t="s">
@@ -8036,16 +8036,16 @@
     </row>
     <row r="314" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B314" s="7">
         <v>157</v>
       </c>
       <c r="C314" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D314" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E314" s="7"/>
       <c r="F314" s="12" t="s">
@@ -8057,16 +8057,16 @@
     </row>
     <row r="315" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B315" s="7">
         <v>158</v>
       </c>
       <c r="C315" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D315" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E315" s="7"/>
       <c r="F315" s="12" t="s">
@@ -8078,16 +8078,16 @@
     </row>
     <row r="316" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B316" s="7">
         <v>159</v>
       </c>
       <c r="C316" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D316" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E316" s="7"/>
       <c r="F316" s="12" t="s">
@@ -8099,16 +8099,16 @@
     </row>
     <row r="317" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B317" s="7">
         <v>160</v>
       </c>
       <c r="C317" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D317" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E317" s="7"/>
       <c r="F317" s="12" t="s">
@@ -8120,16 +8120,16 @@
     </row>
     <row r="318" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B318" s="7">
         <v>161</v>
       </c>
       <c r="C318" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D318" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E318" s="7"/>
       <c r="F318" s="12" t="s">
@@ -8141,16 +8141,16 @@
     </row>
     <row r="319" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B319" s="7">
         <v>162</v>
       </c>
       <c r="C319" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D319" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E319" s="7"/>
       <c r="F319" s="12" t="s">
@@ -8162,16 +8162,16 @@
     </row>
     <row r="320" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B320" s="7">
         <v>163</v>
       </c>
       <c r="C320" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D320" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E320" s="7"/>
       <c r="F320" s="12" t="s">
@@ -8183,16 +8183,16 @@
     </row>
     <row r="321" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B321" s="7">
         <v>164</v>
       </c>
       <c r="C321" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D321" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E321" s="7"/>
       <c r="F321" s="12" t="s">
@@ -8204,16 +8204,16 @@
     </row>
     <row r="322" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B322" s="7">
         <v>165</v>
       </c>
       <c r="C322" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D322" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E322" s="7"/>
       <c r="F322" s="12" t="s">
@@ -8225,16 +8225,16 @@
     </row>
     <row r="323" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B323" s="7">
         <v>166</v>
       </c>
       <c r="C323" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D323" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E323" s="7"/>
       <c r="F323" s="12" t="s">
@@ -8258,7 +8258,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8282,15 +8282,15 @@
         <v>14</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
         <v>307</v>
-      </c>
-      <c r="B2" t="s">
-        <v>215</v>
       </c>
       <c r="C2">
         <v>20210511</v>
@@ -8324,16 +8324,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>